<commit_message>
Updated GBDS File | October 2025
</commit_message>
<xml_diff>
--- a/GBDS OCTOBER FILES 2025/CSR MONTH OF OCTOBER.xlsx
+++ b/GBDS OCTOBER FILES 2025/CSR MONTH OF OCTOBER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS OCTOBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9493A299-93A1-44FC-84E5-3488B88F68DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D5D3FB-5C33-470F-A770-EF42140D124A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="12" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | OCTOBER" sheetId="902" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="10-02 R2" sheetId="905" r:id="rId8"/>
     <sheet name="10-02 R3" sheetId="906" r:id="rId9"/>
     <sheet name="(3)" sheetId="907" r:id="rId10"/>
-    <sheet name="10-03 R1" sheetId="908" r:id="rId11"/>
+    <sheet name="10-03 R1 NO TRIP" sheetId="908" r:id="rId11"/>
     <sheet name="10-03 R2" sheetId="909" r:id="rId12"/>
     <sheet name="10-03 R3" sheetId="910" r:id="rId13"/>
     <sheet name="(4)" sheetId="911" r:id="rId14"/>
@@ -57,7 +57,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="6">'10-02 R1'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">'10-02 R2'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="8">'10-02 R3'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">'10-03 R1'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">'10-03 R1 NO TRIP'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'10-03 R2'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'10-03 R3'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'10-04 R1'!$A$1:$V$44</definedName>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="91">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -332,6 +332,33 @@
   </si>
   <si>
     <t>2/12b</t>
+  </si>
+  <si>
+    <t>33/14B</t>
+  </si>
+  <si>
+    <t>9/15B</t>
+  </si>
+  <si>
+    <t>23/23B</t>
+  </si>
+  <si>
+    <t>1/12B</t>
+  </si>
+  <si>
+    <t>18/14B</t>
+  </si>
+  <si>
+    <t>9/21B</t>
+  </si>
+  <si>
+    <t>28/11B</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>5/12B</t>
   </si>
 </sst>
 </file>
@@ -5990,12 +6017,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -6005,11 +6038,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>1</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -6157,12 +6196,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>83</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -6172,22 +6217,34 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>1</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -6197,11 +6254,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -6579,21 +6642,35 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>18</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>28</v>
+      </c>
+      <c r="M24" s="15">
+        <v>6</v>
+      </c>
+      <c r="N24" s="15">
+        <v>832</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>5</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -6744,21 +6821,35 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>14</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>3</v>
+      </c>
+      <c r="M31" s="24">
+        <v>5</v>
+      </c>
+      <c r="N31" s="24">
+        <v>250</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>5</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -6769,21 +6860,35 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>0</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>4</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>25</v>
+      </c>
+      <c r="M32" s="29">
+        <v>1</v>
+      </c>
+      <c r="N32" s="29">
+        <v>582</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -6910,20 +7015,38 @@
         <v>52</v>
       </c>
       <c r="C36" s="49"/>
-      <c r="D36" s="44"/>
+      <c r="D36" s="44">
+        <v>1</v>
+      </c>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="F36" s="45">
+        <v>463</v>
+      </c>
+      <c r="G36" s="45">
+        <v>17</v>
+      </c>
       <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
+      <c r="I36" s="45">
+        <v>2</v>
+      </c>
       <c r="J36" s="45"/>
       <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+      <c r="L36" s="45">
+        <v>26</v>
+      </c>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>24</v>
+      </c>
+      <c r="O36" s="45">
+        <v>4</v>
+      </c>
+      <c r="P36" s="45">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>18</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -7050,20 +7173,38 @@
         <v>53</v>
       </c>
       <c r="C42" s="49"/>
-      <c r="D42" s="44"/>
+      <c r="D42" s="44">
+        <v>1</v>
+      </c>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="F42" s="45">
+        <v>463</v>
+      </c>
+      <c r="G42" s="45">
+        <v>17</v>
+      </c>
       <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
+      <c r="I42" s="45">
+        <v>2</v>
+      </c>
       <c r="J42" s="45"/>
       <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
+      <c r="L42" s="45">
+        <v>26</v>
+      </c>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="N42" s="45">
+        <v>24</v>
+      </c>
+      <c r="O42" s="45">
+        <v>4</v>
+      </c>
+      <c r="P42" s="45">
+        <v>20</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>18</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -7117,7 +7258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B1154B-60EA-4D0E-9582-F55961ED0334}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7472,25 +7613,37 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>88</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="L8" s="15">
+        <v>1</v>
+      </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>3</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>1</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -7639,50 +7792,74 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>87</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="L15" s="24">
+        <v>1</v>
+      </c>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>3</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>1</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>86</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
-      <c r="L16" s="29"/>
+      <c r="L16" s="29">
+        <v>0</v>
+      </c>
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -8065,16 +8242,28 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>239</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="M24" s="15">
+        <v>7</v>
+      </c>
+      <c r="N24" s="15">
+        <v>513</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>8</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -8230,16 +8419,28 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>85</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="M31" s="24">
+        <v>0</v>
+      </c>
+      <c r="N31" s="24">
+        <v>0</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>0</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -8255,16 +8456,28 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>154</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>7</v>
+      </c>
+      <c r="N32" s="29">
+        <v>513</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>8</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -8390,21 +8603,41 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
+      <c r="F36" s="45">
+        <v>686</v>
+      </c>
+      <c r="G36" s="45">
+        <v>1</v>
+      </c>
+      <c r="H36" s="45">
+        <v>4</v>
+      </c>
+      <c r="I36" s="45">
+        <v>7</v>
+      </c>
       <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+      <c r="K36" s="45">
+        <v>4</v>
+      </c>
+      <c r="L36" s="45">
+        <v>1</v>
+      </c>
       <c r="M36" s="45"/>
       <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="O36" s="45">
+        <v>9</v>
+      </c>
+      <c r="P36" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>6</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -8530,21 +8763,41 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
+      <c r="F42" s="45">
+        <v>686</v>
+      </c>
+      <c r="G42" s="45">
+        <v>1</v>
+      </c>
+      <c r="H42" s="45">
+        <v>4</v>
+      </c>
+      <c r="I42" s="45">
+        <v>7</v>
+      </c>
       <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
+      <c r="K42" s="45">
+        <v>4</v>
+      </c>
+      <c r="L42" s="45">
+        <v>1</v>
+      </c>
       <c r="M42" s="45"/>
       <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="O42" s="45">
+        <v>9</v>
+      </c>
+      <c r="P42" s="45">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>6</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>
@@ -38385,8 +38638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1755F37-82D2-45AC-827D-0289C3C7C753}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" topLeftCell="A26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -38940,7 +39193,7 @@
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S15" s="24"/>
       <c r="T15" s="24">
@@ -38977,7 +39230,7 @@
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
       <c r="R16" s="29">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S16" s="29"/>
       <c r="T16" s="59">

</xml_diff>

<commit_message>
GBDS FILES OCTOBER | GBDS UPDATED
</commit_message>
<xml_diff>
--- a/GBDS OCTOBER FILES 2025/CSR MONTH OF OCTOBER.xlsx
+++ b/GBDS OCTOBER FILES 2025/CSR MONTH OF OCTOBER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS OCTOBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBEB45C-C934-4DEC-8A09-CE14F55C70E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BFED68-27F2-40F6-9A0B-011F403F4F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="16" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="20" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | OCTOBER" sheetId="902" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2388" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="106">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -386,6 +386,30 @@
   </si>
   <si>
     <t>6/12B</t>
+  </si>
+  <si>
+    <t>14/15b</t>
+  </si>
+  <si>
+    <t>5/20b</t>
+  </si>
+  <si>
+    <t>8/19b</t>
+  </si>
+  <si>
+    <t>3/12b</t>
+  </si>
+  <si>
+    <t>9/13b</t>
+  </si>
+  <si>
+    <t>7/19b</t>
+  </si>
+  <si>
+    <t>17/8b</t>
+  </si>
+  <si>
+    <t>25/19b</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1181,9 @@
     <xf numFmtId="16" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1182,9 +1209,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4076,45 +4100,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -4325,13 +4349,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -5556,45 +5580,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -5805,13 +5829,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -7115,45 +7139,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -7400,13 +7424,13 @@
       <c r="Q42" s="46">
         <v>18</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -8704,45 +8728,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -8993,13 +9017,13 @@
       <c r="Q42" s="46">
         <v>6</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -10225,45 +10249,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -10474,13 +10498,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -11117,7 +11141,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="29"/>
-      <c r="H16" s="77">
+      <c r="H16" s="68">
         <v>22</v>
       </c>
       <c r="I16" s="29"/>
@@ -11831,45 +11855,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -12116,13 +12140,13 @@
       <c r="Q42" s="46">
         <v>6</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -13348,45 +13372,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -13597,13 +13621,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -13650,7 +13674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553D8408-329A-4AE0-88C6-DC822F1EF3BB}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -14901,45 +14925,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -15198,13 +15222,13 @@
       <c r="Q42" s="46">
         <v>4</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -16430,45 +16454,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -16679,13 +16703,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -17085,12 +17109,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>98</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -17100,11 +17130,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>1</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>2</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -17252,12 +17288,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>99</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -17267,22 +17309,34 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>1</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>1</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="67" t="s">
+        <v>100</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -17292,11 +17346,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59" t="s">
+        <v>79</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -17674,21 +17734,35 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>2</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>40</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" s="15">
+        <v>13</v>
+      </c>
+      <c r="N24" s="15">
+        <v>272</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>10</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -17839,21 +17913,35 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>0</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>1</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>26</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>0</v>
+      </c>
+      <c r="M31" s="24">
+        <v>0</v>
+      </c>
+      <c r="N31" s="24">
+        <v>14</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>2</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -17864,21 +17952,35 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27" t="s">
+        <v>73</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>1</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>14</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="M32" s="29">
+        <v>13</v>
+      </c>
+      <c r="N32" s="29">
+        <v>258</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>8</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -17910,45 +18012,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -18005,20 +18107,46 @@
         <v>52</v>
       </c>
       <c r="C36" s="49"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
+      <c r="D36" s="44">
+        <v>2</v>
+      </c>
+      <c r="E36" s="45">
+        <v>18</v>
+      </c>
+      <c r="F36" s="45">
+        <v>513</v>
+      </c>
+      <c r="G36" s="45">
+        <v>18</v>
+      </c>
+      <c r="H36" s="45">
+        <v>2</v>
+      </c>
+      <c r="I36" s="45">
+        <v>11</v>
+      </c>
+      <c r="J36" s="45">
+        <v>2</v>
+      </c>
+      <c r="K36" s="45">
+        <v>11</v>
+      </c>
+      <c r="L36" s="45">
+        <v>7</v>
+      </c>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>20</v>
+      </c>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>13</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -18145,27 +18273,53 @@
         <v>53</v>
       </c>
       <c r="C42" s="49"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
+      <c r="D42" s="44">
+        <v>2</v>
+      </c>
+      <c r="E42" s="45">
+        <v>18</v>
+      </c>
+      <c r="F42" s="45">
+        <v>513</v>
+      </c>
+      <c r="G42" s="45">
+        <v>18</v>
+      </c>
+      <c r="H42" s="45">
+        <v>2</v>
+      </c>
+      <c r="I42" s="45">
+        <v>11</v>
+      </c>
+      <c r="J42" s="45">
+        <v>2</v>
+      </c>
+      <c r="K42" s="45">
+        <v>11</v>
+      </c>
+      <c r="L42" s="45">
+        <v>7</v>
+      </c>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="N42" s="45">
+        <v>20</v>
+      </c>
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>3</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>13</v>
+      </c>
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -19391,45 +19545,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -19640,13 +19794,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -20047,11 +20201,15 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -20061,11 +20219,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>1</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -20214,11 +20378,15 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>2</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>103</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -20228,22 +20396,32 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>1</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>102</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -20253,11 +20431,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -20640,13 +20824,23 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>40</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>3</v>
+      </c>
+      <c r="M24" s="15">
+        <v>15</v>
+      </c>
+      <c r="N24" s="15">
+        <v>457</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
@@ -20805,13 +20999,23 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>21</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>3</v>
+      </c>
+      <c r="M31" s="24">
+        <v>9</v>
+      </c>
+      <c r="N31" s="24">
+        <v>185</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
       <c r="Q31" s="24"/>
@@ -20830,13 +21034,23 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>19</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>6</v>
+      </c>
+      <c r="N32" s="29">
+        <v>272</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
@@ -20871,45 +21085,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -20968,16 +21182,36 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
+      <c r="F36" s="45">
+        <v>236</v>
+      </c>
+      <c r="G36" s="45">
+        <v>1</v>
+      </c>
+      <c r="H36" s="45">
+        <v>2</v>
+      </c>
+      <c r="I36" s="45">
+        <v>3</v>
+      </c>
+      <c r="J36" s="45">
+        <v>2</v>
+      </c>
+      <c r="K36" s="45">
+        <v>2</v>
+      </c>
+      <c r="L36" s="45">
+        <v>1</v>
+      </c>
+      <c r="M36" s="45">
+        <v>2</v>
+      </c>
+      <c r="N36" s="45">
+        <v>9</v>
+      </c>
+      <c r="O36" s="45">
+        <v>8</v>
+      </c>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
       <c r="R36" s="40"/>
@@ -21108,25 +21342,45 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
+      <c r="F42" s="45">
+        <v>236</v>
+      </c>
+      <c r="G42" s="45">
+        <v>1</v>
+      </c>
+      <c r="H42" s="45">
+        <v>2</v>
+      </c>
+      <c r="I42" s="45">
+        <v>3</v>
+      </c>
+      <c r="J42" s="45">
+        <v>2</v>
+      </c>
+      <c r="K42" s="45">
+        <v>2</v>
+      </c>
+      <c r="L42" s="45">
+        <v>1</v>
+      </c>
+      <c r="M42" s="45">
+        <v>2</v>
+      </c>
+      <c r="N42" s="45">
+        <v>9</v>
+      </c>
+      <c r="O42" s="45">
+        <v>8</v>
+      </c>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -21173,7 +21427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2368E232-4793-4D8E-97ED-9F3B02BA92CE}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -21528,25 +21782,37 @@
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <v>2</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>105</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="L8" s="15">
+        <v>1</v>
+      </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>3</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>1</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -21695,50 +21961,74 @@
         <v>25</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24">
+        <v>17</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="L15" s="24">
+        <v>1</v>
+      </c>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>3</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>1</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="D16" s="61">
+        <v>1</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
-      <c r="L16" s="29"/>
+      <c r="L16" s="29">
+        <v>0</v>
+      </c>
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -22121,16 +22411,28 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>66</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M24" s="15">
+        <v>15</v>
+      </c>
+      <c r="N24" s="15">
+        <v>491</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>9</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -22286,16 +22588,28 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>36</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>0</v>
+      </c>
+      <c r="M31" s="24">
+        <v>5</v>
+      </c>
+      <c r="N31" s="24">
+        <v>260</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>9</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -22311,16 +22625,28 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>3</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>30</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="M32" s="29">
+        <v>10</v>
+      </c>
+      <c r="N32" s="29">
+        <v>231</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -22352,45 +22678,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -22446,21 +22772,45 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
+      <c r="D36" s="44">
+        <v>1</v>
+      </c>
+      <c r="E36" s="45">
+        <v>15</v>
+      </c>
+      <c r="F36" s="45">
+        <v>362</v>
+      </c>
+      <c r="G36" s="45">
+        <v>18</v>
+      </c>
       <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
+      <c r="I36" s="45">
+        <v>14</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>7</v>
+      </c>
+      <c r="L36" s="45">
+        <v>6</v>
+      </c>
+      <c r="M36" s="45">
+        <v>2</v>
+      </c>
       <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
+      <c r="O36" s="45">
+        <v>7</v>
+      </c>
       <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="Q36" s="46">
+        <v>25</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -22586,28 +22936,52 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
+      <c r="D42" s="44">
+        <v>1</v>
+      </c>
+      <c r="E42" s="45">
+        <v>15</v>
+      </c>
+      <c r="F42" s="45">
+        <v>362</v>
+      </c>
+      <c r="G42" s="45">
+        <v>18</v>
+      </c>
       <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
+      <c r="I42" s="45">
+        <v>14</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>7</v>
+      </c>
+      <c r="L42" s="45">
+        <v>6</v>
+      </c>
+      <c r="M42" s="45">
+        <v>2</v>
+      </c>
       <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
+      <c r="O42" s="45">
+        <v>7</v>
+      </c>
       <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="Q42" s="46">
+        <v>25</v>
+      </c>
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -23833,45 +24207,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -24082,13 +24456,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -25313,45 +25687,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -25562,13 +25936,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -26794,45 +27168,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -27043,13 +27417,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -28275,45 +28649,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -28524,13 +28898,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -29756,45 +30130,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -30005,13 +30379,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -31236,45 +31610,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -31485,13 +31859,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -32717,45 +33091,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -32966,13 +33340,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -34198,45 +34572,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -34447,13 +34821,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -35679,45 +36053,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -35928,13 +36302,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -37160,45 +37534,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -37409,13 +37783,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -38641,45 +39015,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -38890,13 +39264,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -40122,45 +40496,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -40371,13 +40745,13 @@
       <c r="O42" s="45"/>
       <c r="P42" s="45"/>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -41650,45 +42024,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -41927,13 +42301,13 @@
       <c r="Q42" s="46">
         <v>8</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -43232,45 +43606,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -43505,13 +43879,13 @@
         <v>1</v>
       </c>
       <c r="Q42" s="46"/>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
@@ -44809,45 +45183,45 @@
       <c r="W33" s="32"/>
     </row>
     <row r="34" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76" t="s">
+      <c r="D34" s="75"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76" t="s">
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="74"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="75"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="74"/>
-      <c r="N34" s="75"/>
-      <c r="O34" s="76" t="s">
+      <c r="M34" s="75"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="68" t="s">
+      <c r="P34" s="75"/>
+      <c r="Q34" s="76"/>
+      <c r="R34" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="S34" s="69"/>
-      <c r="T34" s="69"/>
-      <c r="U34" s="69"/>
-      <c r="V34" s="70"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="70"/>
+      <c r="U34" s="70"/>
+      <c r="V34" s="71"/>
       <c r="W34" s="32"/>
     </row>
     <row r="35" spans="2:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="73"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="53" t="s">
         <v>49</v>
       </c>
@@ -45074,13 +45448,13 @@
       <c r="Q42" s="46">
         <v>13</v>
       </c>
-      <c r="R42" s="71" t="s">
+      <c r="R42" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="71"/>
-      <c r="T42" s="71"/>
-      <c r="U42" s="71"/>
-      <c r="V42" s="71"/>
+      <c r="S42" s="72"/>
+      <c r="T42" s="72"/>
+      <c r="U42" s="72"/>
+      <c r="V42" s="72"/>
     </row>
     <row r="43" spans="2:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>

</xml_diff>